<commit_message>
To drop rows with missing values
</commit_message>
<xml_diff>
--- a/data/names_and_ages_missing_val.xlsx
+++ b/data/names_and_ages_missing_val.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\PySpark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0D0799-9255-417D-8779-B5C8D1620B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E824038-6B93-4ED8-881A-2E3434BA1C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -77,15 +77,9 @@
     <t>Leo</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
     <t>Nathan</t>
   </si>
   <si>
-    <t>Olivia</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
   </si>
   <si>
     <t>Taylor</t>
-  </si>
-  <si>
-    <t>Ulysses</t>
   </si>
   <si>
     <t>Victoria</t>
@@ -266,7 +257,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -576,7 +567,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +584,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,7 +602,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1500,10000)</f>
-        <v>3835</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,7 +617,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D50" ca="1" si="0">RANDBETWEEN(1500,10000)</f>
-        <v>5520</v>
+        <v>6503</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +632,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>5268</v>
+        <v>6914</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,7 +647,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3314</v>
+        <v>8108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,23 +662,13 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>9271</v>
+        <v>5268</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4961</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -701,7 +682,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>6388</v>
+        <v>6035</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,22 +697,19 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>2112</v>
+        <v>7443</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>27</v>
-      </c>
       <c r="C10">
         <v>25</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>6510</v>
+        <v>9129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,13 +719,6 @@
       <c r="B11">
         <v>33</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1652</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -761,7 +732,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>9000</v>
+        <v>6901</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,13 +747,10 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>8362</v>
+        <v>5013</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
       <c r="B14">
         <v>31</v>
       </c>
@@ -791,28 +759,22 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>5180</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>37</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3679</v>
+        <v>5647</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
       <c r="B16">
         <v>24</v>
       </c>
@@ -821,12 +783,12 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>9435</v>
+        <v>7004</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>38</v>
@@ -836,12 +798,12 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>2178</v>
+        <v>7891</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>21</v>
@@ -851,12 +813,12 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>8670</v>
+        <v>8890</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>34</v>
@@ -866,43 +828,34 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>5535</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>4515</v>
+        <v>4916</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>36</v>
       </c>
-      <c r="C21">
-        <v>15</v>
-      </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>9660</v>
+        <v>5554</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
       <c r="B22">
         <v>42</v>
       </c>
@@ -911,12 +864,12 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>5495</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -926,27 +879,24 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>3902</v>
+        <v>6827</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>5663</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>28</v>
@@ -956,12 +906,12 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>1973</v>
+        <v>7977</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>31</v>
@@ -971,12 +921,12 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>5858</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>29</v>
@@ -986,12 +936,12 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>7371</v>
+        <v>5914</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>26</v>
@@ -1001,12 +951,12 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>8156</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>32</v>
@@ -1016,12 +966,12 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>7614</v>
+        <v>9328</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>23</v>
@@ -1031,12 +981,12 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>9529</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>35</v>
@@ -1046,12 +996,12 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>5249</v>
+        <v>6377</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>27</v>
@@ -1061,12 +1011,12 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>6786</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>30</v>
@@ -1076,12 +1026,12 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>4710</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>24</v>
@@ -1091,12 +1041,12 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>9643</v>
+        <v>5986</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>33</v>
@@ -1106,12 +1056,12 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>4820</v>
+        <v>5233</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>36</v>
@@ -1121,12 +1071,12 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>9324</v>
+        <v>6269</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>28</v>
@@ -1136,12 +1086,12 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>6874</v>
+        <v>8994</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>25</v>
@@ -1151,12 +1101,12 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>8050</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>31</v>
@@ -1166,12 +1116,12 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>7371</v>
+        <v>6966</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>22</v>
@@ -1181,12 +1131,12 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>6165</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>37</v>
@@ -1196,12 +1146,12 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>4442</v>
+        <v>7967</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>39</v>
@@ -1211,12 +1161,12 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>3014</v>
+        <v>6861</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>34</v>
@@ -1226,12 +1176,12 @@
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>8927</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>29</v>
@@ -1241,12 +1191,12 @@
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>4066</v>
+        <v>9300</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>41</v>
@@ -1256,12 +1206,12 @@
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>3190</v>
+        <v>6452</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>40</v>
@@ -1271,12 +1221,12 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="0"/>
-        <v>6910</v>
+        <v>9372</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>26</v>
@@ -1286,12 +1236,12 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="0"/>
-        <v>9361</v>
+        <v>9536</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B48">
         <v>30</v>
@@ -1301,12 +1251,12 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="0"/>
-        <v>5269</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>33</v>
@@ -1316,12 +1266,12 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="0"/>
-        <v>6461</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>28</v>
@@ -1331,7 +1281,7 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="0"/>
-        <v>8716</v>
+        <v>6777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>